<commit_message>
Group assignment logic changed
</commit_message>
<xml_diff>
--- a/tournament_results.xlsx
+++ b/tournament_results.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Team1</t>
+          <t>Team name</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -473,7 +473,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -483,7 +483,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Team2</t>
+          <t>Team1-Santhosh,Sudheer</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -503,7 +503,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Team3</t>
+          <t>Team2-Aarsh,Malik</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -523,7 +523,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Team4</t>
+          <t>Team3-Naga,Sanjay Dasari</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -543,7 +543,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Team5</t>
+          <t>Team4-Karthick,Venkat</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -553,7 +553,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -563,7 +563,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Team6</t>
+          <t>Team5-Manjunath,Saket</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -573,7 +573,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -583,7 +583,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Team7</t>
+          <t>Team6-Sachith,V Ganesh</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -603,7 +603,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Team8</t>
+          <t>Team7-Tushar,Vijay</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -623,7 +623,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Team9</t>
+          <t>Team8-Miraj,Icourt</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -643,7 +643,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Team10</t>
+          <t>Team9-Basav,Tamil</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -653,7 +653,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -663,7 +663,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Team11</t>
+          <t>Team10-Vivek,Anand</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -673,7 +673,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -683,7 +683,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Team12</t>
+          <t>Team11-Sai,Elan</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -693,7 +693,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -703,7 +703,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Team13</t>
+          <t>Team12-Aravind,Laxshman</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -713,7 +713,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -723,7 +723,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Team14</t>
+          <t>Team13-Senthil,Praveen</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -733,7 +733,63 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Team14-Suriya,Azar</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Waseem, Girish</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Team15-Waseem,Girish</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Sanjay P, Mahendar</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Team16-Sanjay P,Mahendar</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -748,7 +804,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N43"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -837,49 +893,49 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Team2</t>
+          <t>Team1-Santhosh,Sudheer</t>
         </is>
       </c>
       <c r="D2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Team2-Aarsh,Malik</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>group</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2026-02-07 11:00</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2026-02-07 11:25</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
         <v>11</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Team11</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>group</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>2026-02-02 09:00</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>2026-02-02 09:20</t>
-        </is>
-      </c>
-      <c r="J2" t="n">
-        <v>3</v>
-      </c>
       <c r="K2" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L2" t="n">
         <v>2</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Team2</t>
+          <t>Team1-Santhosh,Sudheer</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -897,15 +953,15 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Team2</t>
+          <t>Team1-Santhosh,Sudheer</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Team14</t>
+          <t>Team3-Naga,Sanjay Dasari</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -920,26 +976,26 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2026-02-02 09:00</t>
+          <t>2026-02-07 11:00</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2026-02-02 09:20</t>
+          <t>2026-02-07 11:25</t>
         </is>
       </c>
       <c r="J3" t="n">
+        <v>11</v>
+      </c>
+      <c r="K3" t="n">
         <v>10</v>
       </c>
-      <c r="K3" t="n">
-        <v>5</v>
-      </c>
       <c r="L3" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>Team14</t>
+          <t>Team3-Naga,Sanjay Dasari</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -957,15 +1013,15 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Team2</t>
+          <t>Team1-Santhosh,Sudheer</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Team6</t>
+          <t>Team4-Karthick,Venkat</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -980,25 +1036,31 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2026-02-02 09:20</t>
+          <t>2026-02-07 11:00</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2026-02-02 09:40</t>
+          <t>2026-02-07 11:25</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
+        <v>10</v>
+      </c>
+      <c r="L4" t="n">
+        <v>2</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Team1-Santhosh,Sudheer</t>
+        </is>
+      </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -1011,15 +1073,15 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Team2</t>
+          <t>Team1-Santhosh,Sudheer</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Team13</t>
+          <t>Team name</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1034,12 +1096,12 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2026-02-02 09:20</t>
+          <t>2026-02-07 11:25</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2026-02-02 09:40</t>
+          <t>2026-02-07 11:50</t>
         </is>
       </c>
       <c r="J5" t="n">
@@ -1048,11 +1110,17 @@
       <c r="K5" t="n">
         <v>0</v>
       </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
+      <c r="L5" t="n">
+        <v>2</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Team1-Santhosh,Sudheer</t>
+        </is>
+      </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -1061,11 +1129,11 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Team2</t>
+          <t>Team2-Aarsh,Malik</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -1073,7 +1141,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Team4</t>
+          <t>Team3-Naga,Sanjay Dasari</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1088,12 +1156,12 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2026-02-02 09:40</t>
+          <t>2026-02-07 11:25</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2026-02-02 10:00</t>
+          <t>2026-02-07 11:50</t>
         </is>
       </c>
       <c r="J6" t="n">
@@ -1102,11 +1170,17 @@
       <c r="K6" t="n">
         <v>0</v>
       </c>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
+      <c r="L6" t="n">
+        <v>3</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Team2-Aarsh,Malik</t>
+        </is>
+      </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -1115,19 +1189,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Team2</t>
+          <t>Team2-Aarsh,Malik</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Team3</t>
+          <t>Team4-Karthick,Venkat</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1142,12 +1216,12 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2026-02-02 09:40</t>
+          <t>2026-02-07 11:25</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>2026-02-02 10:00</t>
+          <t>2026-02-07 11:50</t>
         </is>
       </c>
       <c r="J7" t="n">
@@ -1156,11 +1230,17 @@
       <c r="K7" t="n">
         <v>0</v>
       </c>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
+      <c r="L7" t="n">
+        <v>5</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Team4-Karthick,Venkat</t>
+        </is>
+      </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -1169,19 +1249,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Team11</t>
+          <t>Team2-Aarsh,Malik</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Team14</t>
+          <t>Team name</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1196,12 +1276,12 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2026-02-02 10:00</t>
+          <t>2026-02-07 11:50</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>2026-02-02 10:20</t>
+          <t>2026-02-07 12:15</t>
         </is>
       </c>
       <c r="J8" t="n">
@@ -1210,11 +1290,17 @@
       <c r="K8" t="n">
         <v>0</v>
       </c>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
+      <c r="L8" t="n">
+        <v>3</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Team2-Aarsh,Malik</t>
+        </is>
+      </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -1223,19 +1309,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Team11</t>
+          <t>Team3-Naga,Sanjay Dasari</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Team6</t>
+          <t>Team4-Karthick,Venkat</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1250,12 +1336,12 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2026-02-02 10:00</t>
+          <t>2026-02-07 11:50</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>2026-02-02 10:20</t>
+          <t>2026-02-07 12:15</t>
         </is>
       </c>
       <c r="J9" t="n">
@@ -1264,11 +1350,17 @@
       <c r="K9" t="n">
         <v>0</v>
       </c>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
+      <c r="L9" t="n">
+        <v>4</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Team3-Naga,Sanjay Dasari</t>
+        </is>
+      </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -1277,19 +1369,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Team11</t>
+          <t>Team3-Naga,Sanjay Dasari</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Team13</t>
+          <t>Team name</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1304,12 +1396,12 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2026-02-02 10:20</t>
+          <t>2026-02-07 11:50</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>2026-02-02 10:40</t>
+          <t>2026-02-07 12:15</t>
         </is>
       </c>
       <c r="J10" t="n">
@@ -1318,11 +1410,17 @@
       <c r="K10" t="n">
         <v>0</v>
       </c>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
+      <c r="L10" t="n">
+        <v>4</v>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>Team3-Naga,Sanjay Dasari</t>
+        </is>
+      </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -1331,19 +1429,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Team11</t>
+          <t>Team4-Karthick,Venkat</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Team4</t>
+          <t>Team name</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1358,12 +1456,12 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2026-02-02 10:20</t>
+          <t>2026-02-07 12:15</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>2026-02-02 10:40</t>
+          <t>2026-02-07 12:40</t>
         </is>
       </c>
       <c r="J11" t="n">
@@ -1372,11 +1470,17 @@
       <c r="K11" t="n">
         <v>0</v>
       </c>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
+      <c r="L11" t="n">
+        <v>5</v>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Team4-Karthick,Venkat</t>
+        </is>
+      </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -1385,19 +1489,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Team11</t>
+          <t>Team5-Manjunath,Saket</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Team3</t>
+          <t>Team6-Sachith,V Ganesh</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1407,17 +1511,17 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2026-02-02 10:40</t>
+          <t>2026-02-07 12:15</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>2026-02-02 11:00</t>
+          <t>2026-02-07 12:40</t>
         </is>
       </c>
       <c r="J12" t="n">
@@ -1426,11 +1530,17 @@
       <c r="K12" t="n">
         <v>0</v>
       </c>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
+      <c r="L12" t="n">
+        <v>6</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>Team5-Manjunath,Saket</t>
+        </is>
+      </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -1439,19 +1549,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Team14</t>
+          <t>Team5-Manjunath,Saket</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Team6</t>
+          <t>Team7-Tushar,Vijay</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1461,17 +1571,17 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2026-02-02 10:40</t>
+          <t>2026-02-07 12:15</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>2026-02-02 11:00</t>
+          <t>2026-02-07 12:40</t>
         </is>
       </c>
       <c r="J13" t="n">
@@ -1480,11 +1590,17 @@
       <c r="K13" t="n">
         <v>0</v>
       </c>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
+      <c r="L13" t="n">
+        <v>8</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>Team7-Tushar,Vijay</t>
+        </is>
+      </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -1493,19 +1609,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Team14</t>
+          <t>Team5-Manjunath,Saket</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Team13</t>
+          <t>Team8-Miraj,Icourt</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1515,17 +1631,17 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2026-02-02 11:00</t>
+          <t>2026-02-07 12:40</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>2026-02-02 11:20</t>
+          <t>2026-02-07 13:05</t>
         </is>
       </c>
       <c r="J14" t="n">
@@ -1534,11 +1650,17 @@
       <c r="K14" t="n">
         <v>0</v>
       </c>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
+      <c r="L14" t="n">
+        <v>6</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Team5-Manjunath,Saket</t>
+        </is>
+      </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -1547,19 +1669,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Team14</t>
+          <t>Team6-Sachith,V Ganesh</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Team4</t>
+          <t>Team7-Tushar,Vijay</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1569,17 +1691,17 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2026-02-02 11:00</t>
+          <t>2026-02-07 12:40</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>2026-02-02 11:20</t>
+          <t>2026-02-07 13:05</t>
         </is>
       </c>
       <c r="J15" t="n">
@@ -1588,11 +1710,17 @@
       <c r="K15" t="n">
         <v>0</v>
       </c>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
+      <c r="L15" t="n">
+        <v>7</v>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>Team6-Sachith,V Ganesh</t>
+        </is>
+      </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -1601,19 +1729,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Team14</t>
+          <t>Team6-Sachith,V Ganesh</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Team3</t>
+          <t>Team8-Miraj,Icourt</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1623,17 +1751,17 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2026-02-02 11:20</t>
+          <t>2026-02-07 12:40</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>2026-02-02 11:40</t>
+          <t>2026-02-07 13:05</t>
         </is>
       </c>
       <c r="J16" t="n">
@@ -1642,11 +1770,17 @@
       <c r="K16" t="n">
         <v>0</v>
       </c>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
+      <c r="L16" t="n">
+        <v>7</v>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Team6-Sachith,V Ganesh</t>
+        </is>
+      </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -1655,19 +1789,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Team6</t>
+          <t>Team7-Tushar,Vijay</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Team13</t>
+          <t>Team8-Miraj,Icourt</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1677,17 +1811,17 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2026-02-02 11:20</t>
+          <t>2026-02-07 13:05</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>2026-02-02 11:40</t>
+          <t>2026-02-07 13:30</t>
         </is>
       </c>
       <c r="J17" t="n">
@@ -1696,11 +1830,17 @@
       <c r="K17" t="n">
         <v>0</v>
       </c>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
+      <c r="L17" t="n">
+        <v>8</v>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>Team7-Tushar,Vijay</t>
+        </is>
+      </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -1709,19 +1849,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Team6</t>
+          <t>Team9-Basav,Tamil</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Team4</t>
+          <t>Team10-Vivek,Anand</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1731,17 +1871,17 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2026-02-02 11:40</t>
+          <t>2026-02-07 13:05</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>2026-02-02 12:00</t>
+          <t>2026-02-07 13:30</t>
         </is>
       </c>
       <c r="J18" t="n">
@@ -1750,11 +1890,17 @@
       <c r="K18" t="n">
         <v>0</v>
       </c>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
+      <c r="L18" t="n">
+        <v>10</v>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Team9-Basav,Tamil</t>
+        </is>
+      </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -1763,19 +1909,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Team6</t>
+          <t>Team9-Basav,Tamil</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Team3</t>
+          <t>Team11-Sai,Elan</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1785,17 +1931,17 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2026-02-02 11:40</t>
+          <t>2026-02-07 13:05</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>2026-02-02 12:00</t>
+          <t>2026-02-07 13:30</t>
         </is>
       </c>
       <c r="J19" t="n">
@@ -1804,11 +1950,17 @@
       <c r="K19" t="n">
         <v>0</v>
       </c>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
+      <c r="L19" t="n">
+        <v>12</v>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Team11-Sai,Elan</t>
+        </is>
+      </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -1817,19 +1969,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
+        <v>10</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Team9-Basav,Tamil</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
         <v>13</v>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Team13</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>4</v>
-      </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Team4</t>
+          <t>Team12-Aravind,Laxshman</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1839,17 +1991,17 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2026-02-02 12:00</t>
+          <t>2026-02-07 13:30</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>2026-02-02 12:20</t>
+          <t>2026-02-07 13:55</t>
         </is>
       </c>
       <c r="J20" t="n">
@@ -1858,11 +2010,17 @@
       <c r="K20" t="n">
         <v>0</v>
       </c>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr"/>
+      <c r="L20" t="n">
+        <v>10</v>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>Team9-Basav,Tamil</t>
+        </is>
+      </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -1871,19 +2029,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Team13</t>
+          <t>Team10-Vivek,Anand</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Team3</t>
+          <t>Team11-Sai,Elan</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1893,17 +2051,17 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2026-02-02 12:00</t>
+          <t>2026-02-07 13:30</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>2026-02-02 12:20</t>
+          <t>2026-02-07 13:55</t>
         </is>
       </c>
       <c r="J21" t="n">
@@ -1912,11 +2070,17 @@
       <c r="K21" t="n">
         <v>0</v>
       </c>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
+      <c r="L21" t="n">
+        <v>11</v>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>Team10-Vivek,Anand</t>
+        </is>
+      </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -1925,19 +2089,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Team4</t>
+          <t>Team10-Vivek,Anand</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Team3</t>
+          <t>Team12-Aravind,Laxshman</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1947,17 +2111,17 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2026-02-02 12:20</t>
+          <t>2026-02-07 13:30</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>2026-02-02 12:40</t>
+          <t>2026-02-07 13:55</t>
         </is>
       </c>
       <c r="J22" t="n">
@@ -1966,11 +2130,17 @@
       <c r="K22" t="n">
         <v>0</v>
       </c>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr"/>
+      <c r="L22" t="n">
+        <v>11</v>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>Team10-Vivek,Anand</t>
+        </is>
+      </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -1979,19 +2149,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Team1</t>
+          <t>Team11-Sai,Elan</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Team8</t>
+          <t>Team12-Aravind,Laxshman</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2001,17 +2171,17 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2026-02-02 12:20</t>
+          <t>2026-02-07 13:55</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>2026-02-02 12:40</t>
+          <t>2026-02-07 14:20</t>
         </is>
       </c>
       <c r="J23" t="n">
@@ -2020,11 +2190,17 @@
       <c r="K23" t="n">
         <v>0</v>
       </c>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr"/>
+      <c r="L23" t="n">
+        <v>12</v>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>Team11-Sai,Elan</t>
+        </is>
+      </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -2033,19 +2209,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Team1</t>
+          <t>Team13-Senthil,Praveen</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Team12</t>
+          <t>Team14-Suriya,Azar</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2055,17 +2231,17 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2026-02-02 12:40</t>
+          <t>2026-02-07 13:55</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>2026-02-02 13:00</t>
+          <t>2026-02-07 14:20</t>
         </is>
       </c>
       <c r="J24" t="n">
@@ -2074,11 +2250,17 @@
       <c r="K24" t="n">
         <v>0</v>
       </c>
-      <c r="L24" t="inlineStr"/>
-      <c r="M24" t="inlineStr"/>
+      <c r="L24" t="n">
+        <v>14</v>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>Team13-Senthil,Praveen</t>
+        </is>
+      </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -2087,19 +2269,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Team1</t>
+          <t>Team13-Senthil,Praveen</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Team7</t>
+          <t>Team15-Waseem,Girish</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2109,17 +2291,17 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2026-02-02 12:40</t>
+          <t>2026-02-07 13:55</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2026-02-02 13:00</t>
+          <t>2026-02-07 14:20</t>
         </is>
       </c>
       <c r="J25" t="n">
@@ -2128,11 +2310,17 @@
       <c r="K25" t="n">
         <v>0</v>
       </c>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
+      <c r="L25" t="n">
+        <v>14</v>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>Team13-Senthil,Praveen</t>
+        </is>
+      </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -2141,19 +2329,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Team1</t>
+          <t>Team13-Senthil,Praveen</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Team10</t>
+          <t>Team16-Sanjay P,Mahendar</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2163,17 +2351,17 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2026-02-02 13:00</t>
+          <t>2026-02-07 14:20</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>2026-02-02 13:20</t>
+          <t>2026-02-07 14:45</t>
         </is>
       </c>
       <c r="J26" t="n">
@@ -2182,11 +2370,17 @@
       <c r="K26" t="n">
         <v>0</v>
       </c>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="inlineStr"/>
+      <c r="L26" t="n">
+        <v>17</v>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>Team16-Sanjay P,Mahendar</t>
+        </is>
+      </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -2195,19 +2389,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Team1</t>
+          <t>Team14-Suriya,Azar</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Team5</t>
+          <t>Team15-Waseem,Girish</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2217,17 +2411,17 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2026-02-02 13:00</t>
+          <t>2026-02-07 14:20</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2026-02-02 13:20</t>
+          <t>2026-02-07 14:45</t>
         </is>
       </c>
       <c r="J27" t="n">
@@ -2236,11 +2430,17 @@
       <c r="K27" t="n">
         <v>0</v>
       </c>
-      <c r="L27" t="inlineStr"/>
-      <c r="M27" t="inlineStr"/>
+      <c r="L27" t="n">
+        <v>15</v>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>Team14-Suriya,Azar</t>
+        </is>
+      </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -2249,19 +2449,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Team1</t>
+          <t>Team14-Suriya,Azar</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Team9</t>
+          <t>Team16-Sanjay P,Mahendar</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2271,17 +2471,17 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2026-02-02 13:20</t>
+          <t>2026-02-07 14:20</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2026-02-02 13:40</t>
+          <t>2026-02-07 14:45</t>
         </is>
       </c>
       <c r="J28" t="n">
@@ -2290,11 +2490,17 @@
       <c r="K28" t="n">
         <v>0</v>
       </c>
-      <c r="L28" t="inlineStr"/>
-      <c r="M28" t="inlineStr"/>
+      <c r="L28" t="n">
+        <v>17</v>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>Team16-Sanjay P,Mahendar</t>
+        </is>
+      </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -2303,19 +2509,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Team8</t>
+          <t>Team15-Waseem,Girish</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Team12</t>
+          <t>Team16-Sanjay P,Mahendar</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2325,17 +2531,17 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2026-02-02 13:20</t>
+          <t>2026-02-07 14:45</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2026-02-02 13:40</t>
+          <t>2026-02-07 15:10</t>
         </is>
       </c>
       <c r="J29" t="n">
@@ -2344,11 +2550,17 @@
       <c r="K29" t="n">
         <v>0</v>
       </c>
-      <c r="L29" t="inlineStr"/>
-      <c r="M29" t="inlineStr"/>
+      <c r="L29" t="n">
+        <v>16</v>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>Team15-Waseem,Girish</t>
+        </is>
+      </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -2357,39 +2569,35 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Team8</t>
+          <t>Team1-Santhosh,Sudheer</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Team7</t>
+          <t>Team10-Vivek,Anand</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>group</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
+          <t>quarterfinal</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2026-02-02 13:40</t>
+          <t>2026-02-07 15:40</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2026-02-02 14:00</t>
+          <t>2026-02-07 16:05</t>
         </is>
       </c>
       <c r="J30" t="n">
@@ -2398,11 +2606,17 @@
       <c r="K30" t="n">
         <v>0</v>
       </c>
-      <c r="L30" t="inlineStr"/>
-      <c r="M30" t="inlineStr"/>
+      <c r="L30" t="n">
+        <v>2</v>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>Team1-Santhosh,Sudheer</t>
+        </is>
+      </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -2411,11 +2625,11 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Team8</t>
+          <t>Team3-Naga,Sanjay Dasari</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -2423,27 +2637,23 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Team10</t>
+          <t>Team9-Basav,Tamil</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>group</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
+          <t>quarterfinal</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2026-02-02 13:40</t>
+          <t>2026-02-07 16:05</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2026-02-02 14:00</t>
+          <t>2026-02-07 16:30</t>
         </is>
       </c>
       <c r="J31" t="n">
@@ -2452,11 +2662,17 @@
       <c r="K31" t="n">
         <v>0</v>
       </c>
-      <c r="L31" t="inlineStr"/>
-      <c r="M31" t="inlineStr"/>
+      <c r="L31" t="n">
+        <v>4</v>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>Team3-Naga,Sanjay Dasari</t>
+        </is>
+      </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -2465,39 +2681,35 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Team8</t>
+          <t>Team5-Manjunath,Saket</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Team5</t>
+          <t>Team16-Sanjay P,Mahendar</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>group</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
+          <t>quarterfinal</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2026-02-02 14:00</t>
+          <t>2026-02-07 16:30</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>2026-02-02 14:20</t>
+          <t>2026-02-07 16:55</t>
         </is>
       </c>
       <c r="J32" t="n">
@@ -2506,11 +2718,17 @@
       <c r="K32" t="n">
         <v>0</v>
       </c>
-      <c r="L32" t="inlineStr"/>
-      <c r="M32" t="inlineStr"/>
+      <c r="L32" t="n">
+        <v>6</v>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>Team5-Manjunath,Saket</t>
+        </is>
+      </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -2519,39 +2737,35 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Team8</t>
+          <t>Team6-Sachith,V Ganesh</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Team9</t>
+          <t>Team13-Senthil,Praveen</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>group</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
+          <t>quarterfinal</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2026-02-02 14:00</t>
+          <t>2026-02-07 16:55</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>2026-02-02 14:20</t>
+          <t>2026-02-07 17:20</t>
         </is>
       </c>
       <c r="J33" t="n">
@@ -2560,11 +2774,17 @@
       <c r="K33" t="n">
         <v>0</v>
       </c>
-      <c r="L33" t="inlineStr"/>
-      <c r="M33" t="inlineStr"/>
+      <c r="L33" t="n">
+        <v>7</v>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>Team6-Sachith,V Ganesh</t>
+        </is>
+      </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -2573,11 +2793,11 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Team12</t>
+          <t>Team1-Santhosh,Sudheer</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -2585,27 +2805,23 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Team7</t>
+          <t>Team6-Sachith,V Ganesh</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>group</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
+          <t>semifinal</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2026-02-02 14:20</t>
+          <t>2026-02-07 17:50</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>2026-02-02 14:40</t>
+          <t>2026-02-07 18:15</t>
         </is>
       </c>
       <c r="J34" t="n">
@@ -2614,11 +2830,17 @@
       <c r="K34" t="n">
         <v>0</v>
       </c>
-      <c r="L34" t="inlineStr"/>
-      <c r="M34" t="inlineStr"/>
+      <c r="L34" t="n">
+        <v>2</v>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>Team1-Santhosh,Sudheer</t>
+        </is>
+      </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -2627,39 +2849,35 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Team12</t>
+          <t>Team3-Naga,Sanjay Dasari</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Team10</t>
+          <t>Team5-Manjunath,Saket</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>group</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
+          <t>semifinal</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2026-02-02 14:20</t>
+          <t>2026-02-07 18:15</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>2026-02-02 14:40</t>
+          <t>2026-02-07 18:40</t>
         </is>
       </c>
       <c r="J35" t="n">
@@ -2668,11 +2886,17 @@
       <c r="K35" t="n">
         <v>0</v>
       </c>
-      <c r="L35" t="inlineStr"/>
-      <c r="M35" t="inlineStr"/>
+      <c r="L35" t="n">
+        <v>4</v>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>Team3-Naga,Sanjay Dasari</t>
+        </is>
+      </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -2681,39 +2905,35 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Team12</t>
+          <t>Team1-Santhosh,Sudheer</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Team5</t>
+          <t>Team3-Naga,Sanjay Dasari</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>group</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
+          <t>final</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2026-02-02 14:40</t>
+          <t>2026-02-07 19:10</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>2026-02-02 15:00</t>
+          <t>2026-02-07 19:30</t>
         </is>
       </c>
       <c r="J36" t="n">
@@ -2722,11 +2942,17 @@
       <c r="K36" t="n">
         <v>0</v>
       </c>
-      <c r="L36" t="inlineStr"/>
-      <c r="M36" t="inlineStr"/>
+      <c r="L36" t="n">
+        <v>2</v>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>Team1-Santhosh,Sudheer</t>
+        </is>
+      </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -2735,41 +2961,29 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Team12</t>
+          <t>Team6-Sachith,V Ganesh</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Team9</t>
+          <t>Team5-Manjunath,Saket</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>group</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>2026-02-02 14:40</t>
-        </is>
-      </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>2026-02-02 15:00</t>
-        </is>
-      </c>
+          <t>third_place</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
       <c r="J37" t="n">
         <v>0</v>
       </c>
@@ -2789,39 +3003,35 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Team7</t>
+          <t>Team1-Santhosh,Sudheer</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Team10</t>
+          <t>Team3-Naga,Sanjay Dasari</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>group</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
+          <t>final</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2026-02-02 15:00</t>
+          <t>2026-02-07 19:30</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>2026-02-02 15:20</t>
+          <t>2026-02-07 19:50</t>
         </is>
       </c>
       <c r="J38" t="n">
@@ -2830,11 +3040,17 @@
       <c r="K38" t="n">
         <v>0</v>
       </c>
-      <c r="L38" t="inlineStr"/>
-      <c r="M38" t="inlineStr"/>
+      <c r="L38" t="n">
+        <v>4</v>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>Team3-Naga,Sanjay Dasari</t>
+        </is>
+      </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>scheduled</t>
+          <t>completed</t>
         </is>
       </c>
     </row>
@@ -2847,37 +3063,25 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Team7</t>
+          <t>Team6-Sachith,V Ganesh</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Team5</t>
+          <t>Team5-Manjunath,Saket</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>group</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>2026-02-02 15:00</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>2026-02-02 15:20</t>
-        </is>
-      </c>
+          <t>third_place</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr"/>
       <c r="J39" t="n">
         <v>0</v>
       </c>
@@ -2887,222 +3091,6 @@
       <c r="L39" t="inlineStr"/>
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr">
-        <is>
-          <t>scheduled</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>39</v>
-      </c>
-      <c r="B40" t="n">
-        <v>7</v>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Team7</t>
-        </is>
-      </c>
-      <c r="D40" t="n">
-        <v>9</v>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>Team9</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>group</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>2026-02-02 15:20</t>
-        </is>
-      </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>2026-02-02 15:40</t>
-        </is>
-      </c>
-      <c r="J40" t="n">
-        <v>0</v>
-      </c>
-      <c r="K40" t="n">
-        <v>0</v>
-      </c>
-      <c r="L40" t="inlineStr"/>
-      <c r="M40" t="inlineStr"/>
-      <c r="N40" t="inlineStr">
-        <is>
-          <t>scheduled</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>40</v>
-      </c>
-      <c r="B41" t="n">
-        <v>10</v>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>Team10</t>
-        </is>
-      </c>
-      <c r="D41" t="n">
-        <v>5</v>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>Team5</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>group</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>2026-02-02 15:20</t>
-        </is>
-      </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>2026-02-02 15:40</t>
-        </is>
-      </c>
-      <c r="J41" t="n">
-        <v>0</v>
-      </c>
-      <c r="K41" t="n">
-        <v>0</v>
-      </c>
-      <c r="L41" t="inlineStr"/>
-      <c r="M41" t="inlineStr"/>
-      <c r="N41" t="inlineStr">
-        <is>
-          <t>scheduled</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>41</v>
-      </c>
-      <c r="B42" t="n">
-        <v>10</v>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Team10</t>
-        </is>
-      </c>
-      <c r="D42" t="n">
-        <v>9</v>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>Team9</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>group</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>2026-02-02 15:40</t>
-        </is>
-      </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>2026-02-02 16:00</t>
-        </is>
-      </c>
-      <c r="J42" t="n">
-        <v>0</v>
-      </c>
-      <c r="K42" t="n">
-        <v>0</v>
-      </c>
-      <c r="L42" t="inlineStr"/>
-      <c r="M42" t="inlineStr"/>
-      <c r="N42" t="inlineStr">
-        <is>
-          <t>scheduled</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>42</v>
-      </c>
-      <c r="B43" t="n">
-        <v>5</v>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>Team5</t>
-        </is>
-      </c>
-      <c r="D43" t="n">
-        <v>9</v>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>Team9</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>group</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>2026-02-02 15:40</t>
-        </is>
-      </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>2026-02-02 16:00</t>
-        </is>
-      </c>
-      <c r="J43" t="n">
-        <v>0</v>
-      </c>
-      <c r="K43" t="n">
-        <v>0</v>
-      </c>
-      <c r="L43" t="inlineStr"/>
-      <c r="M43" t="inlineStr"/>
-      <c r="N43" t="inlineStr">
         <is>
           <t>scheduled</t>
         </is>
@@ -3119,7 +3107,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3205,7 +3193,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Team2</t>
+          <t>Team1-Santhosh,Sudheer</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -3214,34 +3202,34 @@
         </is>
       </c>
       <c r="D2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2" t="n">
+        <v>6</v>
+      </c>
+      <c r="F2" t="n">
         <v>2</v>
       </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I2" t="n">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="J2" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="K2" t="n">
         <v>3</v>
       </c>
       <c r="L2" t="n">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="M2" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="N2" t="n">
         <v>3</v>
@@ -3249,11 +3237,11 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Team14</t>
+          <t>Team3-Naga,Sanjay Dasari</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -3262,94 +3250,94 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I3" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J3" t="n">
+        <v>11</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L3" t="n">
         <v>10</v>
       </c>
-      <c r="K3" t="n">
-        <v>-5</v>
-      </c>
-      <c r="L3" t="n">
-        <v>5</v>
-      </c>
       <c r="M3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N3" t="n">
-        <v>-5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Team2-Aarsh,Malik</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>4</v>
+      </c>
+      <c r="I4" t="n">
+        <v>10</v>
+      </c>
+      <c r="J4" t="n">
         <v>11</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Team11</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>5</v>
-      </c>
-      <c r="J4" t="n">
-        <v>3</v>
-      </c>
       <c r="K4" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="L4" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="M4" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="N4" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Team3</t>
+          <t>Team4-Karthick,Venkat</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -3358,61 +3346,61 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Team name</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Team4</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -3445,28 +3433,28 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Team6</t>
+          <t>Team5-Manjunath,Saket</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -3489,32 +3477,32 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Team13</t>
+          <t>Team6-Sachith,V Ganesh</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -3537,32 +3525,32 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Team7-Tushar,Vijay</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" t="n">
         <v>1</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Team1</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
       <c r="G9" t="n">
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -3585,11 +3573,11 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Team5</t>
+          <t>Team8-Miraj,Icourt</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -3598,13 +3586,13 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -3633,32 +3621,32 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Team7</t>
+          <t>Team9-Basav,Tamil</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
@@ -3681,32 +3669,32 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Team8</t>
+          <t>Team10-Vivek,Anand</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I12" t="n">
         <v>0</v>
@@ -3729,32 +3717,32 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Team9</t>
+          <t>Team11-Sai,Elan</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
@@ -3777,26 +3765,26 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Team10</t>
+          <t>Team12-Aravind,Laxshman</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -3825,32 +3813,32 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Team12</t>
+          <t>Team13-Senthil,Praveen</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -3868,6 +3856,150 @@
         <v>0</v>
       </c>
       <c r="N15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>17</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Team16-Sanjay P,Mahendar</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>4</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>4</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Team14-Suriya,Azar</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>3</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" t="n">
+        <v>2</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>2</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Team15-Waseem,Girish</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>3</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>2</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>